<commit_message>
QA Compiler: Add 4-of-6 column fallback for Item category
When STRINGID is not available for Item category:
1. Try STRINGID matching first
2. Fallback: match by 4+ of first 6 columns matching

This handles sorted files even without STRINGID column.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/Masterfolder_EN/Master_Quest.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/Masterfolder_EN/Master_Quest.xlsx
@@ -835,7 +835,7 @@
         </is>
       </c>
     </row>
-    <row r="6" hidden="1">
+    <row r="6">
       <c r="A6" t="inlineStr">
         <is>
           <t>패배</t>
@@ -859,10 +859,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" promptTitle="Manager Status" prompt="Select status: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
+    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
       <formula1>"FIXED,REPORTED,CHECKING,NON-ISSUE"</formula1>
     </dataValidation>
-    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" promptTitle="Manager Status" prompt="Select status: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
+    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
       <formula1>"FIXED,REPORTED,CHECKING,NON-ISSUE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
QA Compiler: Fix data validation range to prevent Excel repair warnings
- Changed hardcoded row 1000 to actual max_row + 50 buffer
- Prevents Excel from flagging validation on thousands of empty rows
- Applied to both STATUS column creation paths

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/Masterfolder_EN/Master_Quest.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/Masterfolder_EN/Master_Quest.xlsx
@@ -894,10 +894,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
+    <dataValidation sqref="F2:F60" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
       <formula1>"FIXED,REPORTED,CHECKING,NON-ISSUE"</formula1>
     </dataValidation>
-    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
+    <dataValidation sqref="I2:I60" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
       <formula1>"FIXED,REPORTED,CHECKING,NON-ISSUE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Docs: Complete reorganization + DB abstraction architecture
Major restructure of 179 docs into clean hierarchy:
- docs/architecture/ - System design (6 docs)
- docs/protocols/ - Claude protocols (GDP)
- docs/current/ - Active work (SESSION_CONTEXT, ISSUES_TO_FIX)
- docs/reference/ - cicd, enterprise, security
- docs/guides/ - tools, getting-started
- docs/archive/ - 134 historical docs

Key updates:
- Added DB abstraction layer design to ARCHITECTURE_SUMMARY
- Updated OFFLINE_ONLINE_MODE for full offline TM support
- Created docs/INDEX.md as navigation hub
- Fixed all broken links from old wip/ paths
- Added Granular Debug Protocol (GDP) documentation

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/Masterfolder_EN/Master_Quest.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/Masterfolder_EN/Master_Quest.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,9 +36,17 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="002E7D32"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FF8C00"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -78,8 +86,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="0090EE90"/>
         <bgColor rgb="0090EE90"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E8F5E9"/>
+        <bgColor rgb="00E8F5E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE4B5"/>
+        <bgColor rgb="00FFE4B5"/>
       </patternFill>
     </fill>
     <fill>
@@ -95,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -130,6 +156,20 @@
       </top>
       <bottom style="medium">
         <color rgb="004472C4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="00808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="00808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00808080"/>
       </bottom>
     </border>
     <border>
@@ -170,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -196,11 +236,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -212,10 +252,19 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -698,7 +747,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -713,11 +762,13 @@
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
     <col width="35" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="40" customWidth="1" min="8" max="8"/>
-    <col hidden="1" width="35" customWidth="1" min="9" max="9"/>
-    <col hidden="1" width="15" customWidth="1" min="10" max="10"/>
-    <col hidden="1" width="40" customWidth="1" min="11" max="11"/>
+    <col hidden="1" width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="40" customWidth="1" min="9" max="9"/>
+    <col width="35" customWidth="1" min="10" max="10"/>
+    <col hidden="1" width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="40" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -753,31 +804,41 @@
       </c>
       <c r="G1" s="14" t="inlineStr">
         <is>
+          <t>TESTER_STATUS_Eric</t>
+        </is>
+      </c>
+      <c r="H1" s="15" t="inlineStr">
+        <is>
           <t>STATUS_Eric</t>
         </is>
       </c>
-      <c r="H1" s="13" t="inlineStr">
+      <c r="I1" s="13" t="inlineStr">
         <is>
           <t>SCREENSHOT_Eric</t>
         </is>
       </c>
-      <c r="I1" s="13" t="inlineStr">
+      <c r="J1" s="13" t="inlineStr">
         <is>
           <t>COMMENT_John</t>
         </is>
       </c>
-      <c r="J1" s="14" t="inlineStr">
+      <c r="K1" s="14" t="inlineStr">
+        <is>
+          <t>TESTER_STATUS_John</t>
+        </is>
+      </c>
+      <c r="L1" s="15" t="inlineStr">
         <is>
           <t>STATUS_John</t>
         </is>
       </c>
-      <c r="K1" s="13" t="inlineStr">
+      <c r="M1" s="13" t="inlineStr">
         <is>
           <t>SCREENSHOT_John</t>
         </is>
       </c>
     </row>
-    <row r="2" hidden="1" ht="15" customHeight="1">
+    <row r="2" hidden="1" ht="75" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Prologue. 깊은 밤</t>
@@ -795,14 +856,40 @@
       </c>
       <c r="D2" s="2" t="n"/>
       <c r="E2" s="2" t="n"/>
-      <c r="F2" s="15" t="n"/>
-      <c r="G2" s="15" t="n"/>
-      <c r="H2" s="15" t="n"/>
-      <c r="I2" s="15" t="n"/>
-      <c r="J2" s="15" t="n"/>
-      <c r="K2" s="15" t="n"/>
+      <c r="F2" s="16" t="inlineStr">
+        <is>
+          <t>Typo in Korean text
+---
+stringid:
+1887229000892285192
+(updated: 260109 1556)</t>
+        </is>
+      </c>
+      <c r="G2" s="17" t="inlineStr">
+        <is>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="H2" s="17" t="n"/>
+      <c r="I2" s="17" t="n"/>
+      <c r="J2" s="16" t="inlineStr">
+        <is>
+          <t>Character name inconsistent
+---
+stringid:
+1887229000892285192
+(updated: 260109 1556)</t>
+        </is>
+      </c>
+      <c r="K2" s="17" t="inlineStr">
+        <is>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="L2" s="17" t="n"/>
+      <c r="M2" s="17" t="n"/>
     </row>
-    <row r="3" hidden="1" ht="15" customHeight="1">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Prologue. 깊은 밤</t>
@@ -824,14 +911,16 @@
         </is>
       </c>
       <c r="E3" s="4" t="n"/>
-      <c r="F3" s="15" t="n"/>
-      <c r="G3" s="15" t="n"/>
-      <c r="H3" s="15" t="n"/>
-      <c r="I3" s="15" t="n"/>
-      <c r="J3" s="15" t="n"/>
-      <c r="K3" s="15" t="n"/>
+      <c r="F3" s="17" t="n"/>
+      <c r="G3" s="17" t="n"/>
+      <c r="H3" s="17" t="n"/>
+      <c r="I3" s="17" t="n"/>
+      <c r="J3" s="17" t="n"/>
+      <c r="K3" s="17" t="n"/>
+      <c r="L3" s="17" t="n"/>
+      <c r="M3" s="17" t="n"/>
     </row>
-    <row r="4" hidden="1" ht="30" customHeight="1">
+    <row r="4" ht="75" customHeight="1">
       <c r="A4" s="6" t="inlineStr">
         <is>
           <t>오두막으로 이동하기</t>
@@ -858,14 +947,32 @@
 /teleport -9912.28 625.15 -2807</t>
         </is>
       </c>
-      <c r="F4" s="15" t="n"/>
-      <c r="G4" s="15" t="n"/>
-      <c r="H4" s="15" t="n"/>
-      <c r="I4" s="15" t="n"/>
-      <c r="J4" s="15" t="n"/>
-      <c r="K4" s="15" t="n"/>
+      <c r="F4" s="18" t="inlineStr">
+        <is>
+          <t>Need context for this French text
+---
+stringid:
+11417051416787681537
+(updated: 260109 1556)</t>
+        </is>
+      </c>
+      <c r="G4" s="17" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
+      <c r="H4" s="17" t="n"/>
+      <c r="I4" s="17" t="n"/>
+      <c r="J4" s="17" t="n"/>
+      <c r="K4" s="17" t="inlineStr">
+        <is>
+          <t>ISSUE</t>
+        </is>
+      </c>
+      <c r="L4" s="17" t="n"/>
+      <c r="M4" s="17" t="n"/>
     </row>
-    <row r="5" hidden="1" ht="15" customHeight="1">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="8" t="inlineStr">
         <is>
           <t>주변 탐색하기</t>
@@ -883,12 +990,18 @@
       </c>
       <c r="D5" s="8" t="n"/>
       <c r="E5" s="8" t="n"/>
-      <c r="F5" s="15" t="n"/>
-      <c r="G5" s="15" t="n"/>
-      <c r="H5" s="15" t="n"/>
-      <c r="I5" s="15" t="n"/>
-      <c r="J5" s="15" t="n"/>
-      <c r="K5" s="15" t="n"/>
+      <c r="F5" s="17" t="n"/>
+      <c r="G5" s="17" t="n"/>
+      <c r="H5" s="17" t="n"/>
+      <c r="I5" s="17" t="n"/>
+      <c r="J5" s="17" t="n"/>
+      <c r="K5" s="17" t="inlineStr">
+        <is>
+          <t>ISSUE</t>
+        </is>
+      </c>
+      <c r="L5" s="17" t="n"/>
+      <c r="M5" s="17" t="n"/>
     </row>
     <row r="6" hidden="1" ht="15" customHeight="1">
       <c r="A6" s="8" t="inlineStr">
@@ -912,14 +1025,20 @@
         </is>
       </c>
       <c r="E6" s="8" t="n"/>
-      <c r="F6" s="15" t="n"/>
-      <c r="G6" s="15" t="n"/>
-      <c r="H6" s="15" t="n"/>
-      <c r="I6" s="15" t="n"/>
-      <c r="J6" s="15" t="n"/>
-      <c r="K6" s="15" t="n"/>
+      <c r="F6" s="17" t="n"/>
+      <c r="G6" s="17" t="n"/>
+      <c r="H6" s="17" t="n"/>
+      <c r="I6" s="17" t="n"/>
+      <c r="J6" s="17" t="n"/>
+      <c r="K6" s="17" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
+      <c r="L6" s="17" t="n"/>
+      <c r="M6" s="17" t="n"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" hidden="1" ht="75" customHeight="1">
       <c r="A7" s="8" t="inlineStr">
         <is>
           <t>마리우스와 대화하기</t>
@@ -937,12 +1056,26 @@
       </c>
       <c r="D7" s="8" t="n"/>
       <c r="E7" s="8" t="n"/>
-      <c r="F7" s="15" t="n"/>
-      <c r="G7" s="15" t="n"/>
-      <c r="H7" s="15" t="n"/>
-      <c r="I7" s="15" t="n"/>
-      <c r="J7" s="15" t="n"/>
-      <c r="K7" s="15" t="n"/>
+      <c r="F7" s="17" t="n"/>
+      <c r="G7" s="17" t="n"/>
+      <c r="H7" s="17" t="n"/>
+      <c r="I7" s="17" t="n"/>
+      <c r="J7" s="18" t="inlineStr">
+        <is>
+          <t>Missing context
+---
+stringid:
+8122573288984543489
+(updated: 260109 1556)</t>
+        </is>
+      </c>
+      <c r="K7" s="17" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
+      <c r="L7" s="17" t="n"/>
+      <c r="M7" s="17" t="n"/>
     </row>
     <row r="8" ht="75" customHeight="1">
       <c r="A8" s="8" t="inlineStr">
@@ -971,7 +1104,7 @@
 /teleport -9912.28 625.15 -2807</t>
         </is>
       </c>
-      <c r="F8" s="16" t="inlineStr">
+      <c r="F8" s="19" t="inlineStr">
         <is>
           <t>Looks good in French
 ---
@@ -980,46 +1113,78 @@
 (updated: 260109 1556)</t>
         </is>
       </c>
-      <c r="G8" s="15" t="n"/>
-      <c r="H8" s="15" t="n"/>
-      <c r="I8" s="15" t="n"/>
-      <c r="J8" s="15" t="n"/>
-      <c r="K8" s="15" t="n"/>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>ISSUE</t>
+        </is>
+      </c>
+      <c r="H8" s="17" t="n"/>
+      <c r="I8" s="17" t="n"/>
+      <c r="J8" s="18" t="inlineStr">
+        <is>
+          <t>Font rendering issue
+---
+stringid:
+6951248150162047233
+(updated: 260109 1556)</t>
+        </is>
+      </c>
+      <c r="K8" s="17" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
+      <c r="L8" s="17" t="n"/>
+      <c r="M8" s="17" t="n"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="15" t="inlineStr">
+    <row r="9" hidden="1" ht="75" customHeight="1">
+      <c r="A9" s="17" t="inlineStr">
         <is>
           <t>루소와 대화하기</t>
         </is>
       </c>
-      <c r="B9" s="15" t="inlineStr">
+      <c r="B9" s="17" t="inlineStr">
         <is>
           <t>Talk to Ross</t>
         </is>
       </c>
-      <c r="C9" s="15" t="inlineStr">
+      <c r="C9" s="17" t="inlineStr">
         <is>
           <t>Parler à Ross</t>
         </is>
       </c>
-      <c r="D9" s="15" t="n"/>
-      <c r="E9" s="15" t="n"/>
-      <c r="F9" s="15" t="n"/>
-      <c r="G9" s="15" t="n"/>
-      <c r="H9" s="15" t="n"/>
-      <c r="I9" s="15" t="n"/>
-      <c r="J9" s="15" t="n"/>
-      <c r="K9" s="15" t="n"/>
+      <c r="D9" s="17" t="n"/>
+      <c r="E9" s="17" t="n"/>
+      <c r="F9" s="17" t="n"/>
+      <c r="G9" s="17" t="n"/>
+      <c r="H9" s="17" t="n"/>
+      <c r="I9" s="17" t="n"/>
+      <c r="J9" s="18" t="inlineStr">
+        <is>
+          <t>Punctuation error
+---
+stringid:
+14797137245051552001
+(updated: 260109 1556)</t>
+        </is>
+      </c>
+      <c r="K9" s="17" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
+      <c r="L9" s="17" t="n"/>
+      <c r="M9" s="17" t="n"/>
     </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation sqref="F2:F8" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"ISSUE,NO ISSUE,BLOCKED"</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G60" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" promptTitle="Manager Status" prompt="Select status: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
+    <dataValidation sqref="H2:H60" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" promptTitle="Manager Status" prompt="Select status: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
       <formula1>"FIXED,REPORTED,CHECKING,NON-ISSUE"</formula1>
     </dataValidation>
-    <dataValidation sqref="J2:J60" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" promptTitle="Manager Status" prompt="Select status: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
+    <dataValidation sqref="L2:L60" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Status" error="Please select: FIXED, REPORTED, CHECKING, or NON-ISSUE" promptTitle="Manager Status" prompt="Select status: FIXED, REPORTED, CHECKING, or NON-ISSUE" type="list">
       <formula1>"FIXED,REPORTED,CHECKING,NON-ISSUE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>